<commit_message>
Final Version -full function as needed-
</commit_message>
<xml_diff>
--- a/input/myData.xlsx
+++ b/input/myData.xlsx
@@ -19,25 +19,25 @@
     <t>Location</t>
   </si>
   <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Tolip Hotel Alexandria</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Check-in date</t>
+  </si>
+  <si>
     <t>Check-out date</t>
   </si>
   <si>
-    <t>Check-in date</t>
-  </si>
-  <si>
-    <t>Desired hotel</t>
-  </si>
-  <si>
-    <t>Alexandria</t>
-  </si>
-  <si>
-    <t>01 October 2023</t>
-  </si>
-  <si>
-    <t>15 October 2023</t>
-  </si>
-  <si>
-    <t>Tolip Hotel Alexandria</t>
+    <t>9 October 2023</t>
+  </si>
+  <si>
+    <t>30 October 2023</t>
   </si>
 </sst>
 </file>
@@ -94,10 +94,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,13 +402,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -409,28 +417,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Version with assertions
</commit_message>
<xml_diff>
--- a/input/myData.xlsx
+++ b/input/myData.xlsx
@@ -34,16 +34,20 @@
     <t>Check-out date</t>
   </si>
   <si>
-    <t>9 October 2023</t>
-  </si>
-  <si>
-    <t>30 October 2023</t>
+    <t>1 October 2023</t>
+  </si>
+  <si>
+    <t>14 October 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -94,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -105,6 +109,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,9 +419,10 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,19 +436,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>